<commit_message>
Parte renovacion de licencias
</commit_message>
<xml_diff>
--- a/Registros de Prueba.xlsx
+++ b/Registros de Prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unitechn-my.sharepoint.com/personal/hailtonamaya_unitec_edu/Documents/Intro a Ciencia de Datos/Programas_de_Clase/ProyectoCDIA/ProyectoIntroCDIA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{E52D1DD7-360B-41CE-8037-CAD540F02047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C88BCB5-9CD9-420C-8A87-1D9FD44977DC}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{E52D1DD7-360B-41CE-8037-CAD540F02047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AFC84D8-5670-49F8-9BE8-88F777755E7A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{52728D16-9ED0-441C-9C9A-D719E3FF4BC2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>Nombre</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Carlos Aguilar</t>
+  </si>
+  <si>
+    <t>0501200525258</t>
   </si>
 </sst>
 </file>
@@ -151,12 +154,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -174,6 +180,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -496,7 +506,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -589,14 +599,14 @@
       <c r="B3" s="2">
         <v>18</v>
       </c>
-      <c r="C3" s="2">
-        <v>501200525258</v>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>13</v>
@@ -958,6 +968,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="C2" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>